<commit_message>
cleaning up for opensource and adding clean outputs for analysis for future modeling
</commit_message>
<xml_diff>
--- a/Inputs/two_degree/energyScenerio_IEABeyond2Degree.xlsx
+++ b/Inputs/two_degree/energyScenerio_IEABeyond2Degree.xlsx
@@ -85,7 +85,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -117,12 +117,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -444,24 +441,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="5" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="5" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="5" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="5" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="5" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="4" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="4" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="4" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="4" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="4" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="4" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="4" width="24.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="4" width="17.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
@@ -520,1179 +517,1179 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1">
         <v>2000</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>446.9034441</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>1142.99277</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>796.5261604</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>351.483</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>32.615</v>
       </c>
       <c r="I2" s="1">
         <v>0</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>686.363</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="2">
         <v>8.3223</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="2">
         <v>17.254</v>
       </c>
       <c r="M2" s="1">
         <v>0</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="2">
         <v>0.9873</v>
       </c>
       <c r="O2" s="1">
         <v>0</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="2">
         <v>0.4774</v>
       </c>
       <c r="Q2" s="1">
         <v>0</v>
       </c>
-      <c r="R2" s="3">
+      <c r="R2" s="2">
         <v>0.23935796904997067</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1">
         <v>2001</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>444.3440191</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>1161.53176</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>857.9635087</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>354.507</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>34.973</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="2">
         <v>696.115</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="2">
         <v>8.1193</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="2">
         <v>23.858</v>
       </c>
       <c r="M3" s="1">
         <v>0</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="2">
         <v>1.2302</v>
       </c>
       <c r="O3" s="1">
         <v>0</v>
       </c>
-      <c r="P3" s="3">
+      <c r="P3" s="2">
         <v>0.4259</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="Q3" s="2">
         <v>0.362865</v>
       </c>
-      <c r="R3" s="3">
+      <c r="R3" s="2">
         <v>-0.02826309013048195</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1">
         <v>2002</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>443.8765981</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>1178.77253</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>953.118875</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>359.873</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>36.883</v>
       </c>
       <c r="I4" s="1">
         <v>0</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>710.837</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <v>8.1683</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <v>30.822</v>
       </c>
       <c r="M4" s="1">
         <v>0</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="2">
         <v>1.5197</v>
       </c>
       <c r="O4" s="1">
         <v>0</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4" s="2">
         <v>0.4869</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q4" s="2">
         <v>0.725731</v>
       </c>
-      <c r="R4" s="3">
+      <c r="R4" s="2">
         <v>-0.2579862303869908</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1">
         <v>2003</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>444.0773591</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>1200.78483</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>1032.630843</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>361.918</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>39.048</v>
       </c>
       <c r="I5" s="1">
         <v>0</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>730.474</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <v>8.2993</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="2">
         <v>38.524</v>
       </c>
       <c r="M5" s="1">
         <v>0</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="2">
         <v>1.9997</v>
       </c>
       <c r="O5" s="1">
         <v>0</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="2">
         <v>0.9699</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5" s="2">
         <v>1.088596</v>
       </c>
-      <c r="R5" s="3">
+      <c r="R5" s="2">
         <v>-0.4347289327568098</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1">
         <v>2004</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>437.7829091</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>1232.10895</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>1084.2908</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>366.573</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>41.878</v>
       </c>
       <c r="I6" s="1">
         <v>0</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <v>745.517</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="2">
         <v>8.2823</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="2">
         <v>47.018</v>
       </c>
       <c r="M6" s="1">
         <v>0</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="2">
         <v>3.0081</v>
       </c>
       <c r="O6" s="1">
         <v>0</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6" s="2">
         <v>1.0079</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="Q6" s="2">
         <v>1.451462</v>
       </c>
-      <c r="R6" s="3">
+      <c r="R6" s="2">
         <v>-0.5374119252574446</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1">
         <v>2005</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>436.1078931</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>1282.35613</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>1128.689139</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>370.186</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>47.9091</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <v>757.599</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="2">
         <v>8.6731</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="2">
         <v>59.3427</v>
       </c>
       <c r="M7" s="1">
         <v>0</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="2">
         <v>4.4291</v>
       </c>
       <c r="O7" s="1">
         <v>0</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7" s="2">
         <v>1.2519</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="Q7" s="2">
         <v>1.814327</v>
       </c>
-      <c r="R7" s="3">
+      <c r="R7" s="2">
         <v>-0.5365633978974773</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1">
         <v>2006</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>433.7099481</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>1371.43078</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>1175.210918</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>371.672</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>52.18851</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <v>781.167</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="2">
         <v>8.8683</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="2">
         <v>73.0877</v>
       </c>
       <c r="M8" s="1">
         <v>0</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="2">
         <v>5.7965</v>
       </c>
       <c r="O8" s="1">
         <v>0</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8" s="2">
         <v>1.4299</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="Q8" s="2">
         <v>2.177193</v>
       </c>
-      <c r="R8" s="3">
+      <c r="R8" s="2">
         <v>-0.3909890840735526</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1">
         <v>2007</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>431.5899541</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>1438.10239</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>1216.895221</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>371.621</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>54.8026</v>
       </c>
       <c r="I9" s="1">
         <v>0</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <v>806.631</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="2">
         <v>9.0693</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="2">
         <v>91.66553</v>
       </c>
       <c r="M9" s="1">
         <v>0</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="2">
         <v>8.196</v>
       </c>
       <c r="O9" s="1">
         <v>0</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9" s="2">
         <v>1.1835</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="Q9" s="2">
         <v>2.540058</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R9" s="2">
         <v>-0.04309813667233975</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1">
         <v>2008</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>431.4216531</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>1503.1098</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>1257.403639</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>371.626</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>60.39709</v>
       </c>
       <c r="I10" s="1">
         <v>0</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <v>833.562</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="2">
         <v>9.3733</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="2">
         <v>116.20753</v>
       </c>
       <c r="M10" s="1">
         <v>0</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="2">
         <v>14.0818</v>
       </c>
       <c r="O10" s="1">
         <v>0</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10" s="2">
         <v>1.1935</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="Q10" s="2">
         <v>2.902924</v>
       </c>
-      <c r="R10" s="3">
+      <c r="R10" s="2">
         <v>0.587611712903469</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1">
         <v>2009</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>433.5205631</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>1566.74895</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>1311.836717</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>370.9347</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>67.97138</v>
       </c>
       <c r="I11" s="1">
         <v>0</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <v>863.1667</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="2">
         <v>9.8663</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11" s="2">
         <v>149.95435</v>
       </c>
       <c r="M11" s="1">
         <v>0</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="2">
         <v>21.8539</v>
       </c>
       <c r="O11" s="1">
         <v>0</v>
       </c>
-      <c r="P11" s="3">
+      <c r="P11" s="2">
         <v>1.224</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="Q11" s="2">
         <v>3.265789</v>
       </c>
-      <c r="R11" s="3">
+      <c r="R11" s="2">
         <v>1.6136805269219545</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1">
         <v>2010</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>438.6404551</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>1628.329519</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>1370.852966</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>375.2204</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>74.51978</v>
       </c>
       <c r="I12" s="1">
         <v>0</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="2">
         <v>892.2867</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="2">
         <v>10.108</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="2">
         <v>180.39437</v>
       </c>
       <c r="M12" s="1">
         <v>0</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12" s="2">
         <v>38.2664</v>
       </c>
       <c r="O12" s="1">
         <v>0</v>
       </c>
-      <c r="P12" s="3">
+      <c r="P12" s="2">
         <v>1.24</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="Q12" s="2">
         <v>3.628655</v>
       </c>
-      <c r="R12" s="3">
+      <c r="R12" s="2">
         <v>1.7502918022161253</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1">
         <v>2011</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>444.4863071</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>1713.500653</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>1420.075538</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <v>368.7118</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="2">
         <v>81.3384</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="2">
         <v>917.5166</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13" s="2">
         <v>10.0356</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13" s="2">
         <v>219.86107</v>
       </c>
       <c r="M13" s="1">
         <v>0</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13" s="2">
         <v>67.9903</v>
       </c>
       <c r="O13" s="1">
         <v>0</v>
       </c>
-      <c r="P13" s="3">
+      <c r="P13" s="2">
         <v>1.2683</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="Q13" s="2">
         <v>3.99152</v>
       </c>
-      <c r="R13" s="3">
+      <c r="R13" s="2">
         <v>6.766373604432253</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1">
         <v>2012</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>441.6267281</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>1772.576138</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>1473.350752</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
         <v>372.617</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
         <v>87.5506</v>
       </c>
       <c r="I14" s="1">
         <v>0</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="2">
         <v>945.301</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="2">
         <v>10.4865</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14" s="2">
         <v>268.3731</v>
       </c>
       <c r="M14" s="1">
         <v>0</v>
       </c>
-      <c r="N14" s="3">
+      <c r="N14" s="2">
         <v>95.2801</v>
       </c>
       <c r="O14" s="1">
         <v>0</v>
       </c>
-      <c r="P14" s="3">
+      <c r="P14" s="2">
         <v>1.1897</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="Q14" s="2">
         <v>13.7218</v>
       </c>
-      <c r="R14" s="3">
+      <c r="R14" s="2">
         <v>0.878198463158057</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1">
         <v>2013</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>438.6102581</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>1821.156142</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>1512.548369</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="2">
         <v>371.9533</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="2">
         <v>94.646</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="2">
         <v>990.116</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15" s="2">
         <v>10.7784</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15" s="2">
         <v>302.5887</v>
       </c>
       <c r="M15" s="1">
         <v>0</v>
       </c>
-      <c r="N15" s="3">
+      <c r="N15" s="2">
         <v>131.1742</v>
       </c>
       <c r="O15" s="1">
         <v>0</v>
       </c>
-      <c r="P15" s="3">
+      <c r="P15" s="2">
         <v>1.5877</v>
       </c>
-      <c r="Q15" s="3">
+      <c r="Q15" s="2">
         <v>13.7218</v>
       </c>
-      <c r="R15" s="3">
+      <c r="R15" s="2">
         <v>7.793987208864506</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1">
         <v>2014</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>441.5868341</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>1889.093867</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>1574.537682</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="2">
         <v>333.7583</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="2">
         <v>100.9731</v>
       </c>
       <c r="I16" s="1">
         <v>0</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="2">
         <v>1027.3073</v>
       </c>
-      <c r="K16" s="3">
+      <c r="K16" s="2">
         <v>11.3707</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L16" s="2">
         <v>340.2338</v>
       </c>
       <c r="M16" s="1">
         <v>9</v>
       </c>
-      <c r="N16" s="3">
+      <c r="N16" s="2">
         <v>169.9519</v>
       </c>
       <c r="O16" s="1">
         <v>4</v>
       </c>
-      <c r="P16" s="3">
+      <c r="P16" s="2">
         <v>1.6934</v>
       </c>
-      <c r="Q16" s="3">
+      <c r="Q16" s="2">
         <v>13.7218</v>
       </c>
-      <c r="R16" s="3">
+      <c r="R16" s="2">
         <v>15.093986440443535</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1">
         <v>2015</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>441.3899561</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>1963.899891</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>1614.941119</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="2">
         <v>343.215</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="2">
         <v>106.7497</v>
       </c>
       <c r="I17" s="1">
         <v>0</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="2">
         <v>1058.6052</v>
       </c>
-      <c r="K17" s="3">
+      <c r="K17" s="2">
         <v>11.8239</v>
       </c>
-      <c r="L17" s="3">
+      <c r="L17" s="2">
         <v>405.7657</v>
       </c>
       <c r="M17" s="1">
         <v>9</v>
       </c>
-      <c r="N17" s="3">
+      <c r="N17" s="2">
         <v>217.07513333333333</v>
       </c>
-      <c r="O17" s="3">
+      <c r="O17" s="2">
         <v>4.376666666666667</v>
       </c>
-      <c r="P17" s="3">
+      <c r="P17" s="2">
         <v>1.6691</v>
       </c>
-      <c r="Q17" s="3">
+      <c r="Q17" s="2">
         <v>13.7218</v>
       </c>
-      <c r="R17" s="3">
+      <c r="R17" s="2">
         <v>18.936091299169334</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1">
         <v>2016</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>445.9714371</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>2025.071006</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>1643.629117</v>
       </c>
       <c r="F18" s="1">
         <v>0</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="2">
         <v>352.8238</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="2">
         <v>116.2517</v>
       </c>
       <c r="I18" s="1">
         <v>0</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="2">
         <v>1086.7059</v>
       </c>
-      <c r="K18" s="3">
+      <c r="K18" s="2">
         <v>12.247</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18" s="2">
         <v>458.8069</v>
       </c>
       <c r="M18" s="1">
         <v>9</v>
       </c>
-      <c r="N18" s="3">
+      <c r="N18" s="2">
         <v>290.31596666666667</v>
       </c>
-      <c r="O18" s="3">
+      <c r="O18" s="2">
         <v>4.753333333333334</v>
       </c>
-      <c r="P18" s="3">
+      <c r="P18" s="2">
         <v>1.7428</v>
       </c>
-      <c r="Q18" s="3">
+      <c r="Q18" s="2">
         <v>13.7218</v>
       </c>
-      <c r="R18" s="3">
+      <c r="R18" s="2">
         <v>28.92556393185643</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1">
         <v>2017</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>446.6065781</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>2066.73833</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>1694.772895</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="2">
         <v>353.6849</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="2">
         <v>123.342</v>
       </c>
       <c r="I19" s="1">
         <v>0</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="2">
         <v>1100.6565</v>
       </c>
-      <c r="K19" s="3">
+      <c r="K19" s="2">
         <v>12.7407</v>
       </c>
-      <c r="L19" s="3">
+      <c r="L19" s="2">
         <v>505.71220000000005</v>
       </c>
       <c r="M19" s="1">
         <v>9</v>
       </c>
-      <c r="N19" s="3">
+      <c r="N19" s="2">
         <v>382.1129</v>
       </c>
-      <c r="O19" s="3">
+      <c r="O19" s="2">
         <v>5.13</v>
       </c>
-      <c r="P19" s="3">
+      <c r="P19" s="2">
         <v>1.8348</v>
       </c>
-      <c r="Q19" s="3">
+      <c r="Q19" s="2">
         <v>13.7218</v>
       </c>
-      <c r="R19" s="3">
+      <c r="R19" s="2">
         <v>62.351876202770924</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1">
         <v>2018</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>442.173907042534</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>2025.0065370482666</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>0.7254713406453344</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>1731.2885690955943</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>0.22126557315903314</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <v>376.44197787031254</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
         <v>150.40979597709764</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="2">
         <v>0.077830320843074</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="2">
         <v>1139.8831835792964</v>
       </c>
-      <c r="K20" s="3">
+      <c r="K20" s="2">
         <v>15.483091126476406</v>
       </c>
-      <c r="L20" s="3">
+      <c r="L20" s="2">
         <v>586.8871065937074</v>
       </c>
-      <c r="M20" s="3">
+      <c r="M20" s="2">
         <v>15.673899522512553</v>
       </c>
-      <c r="N20" s="3">
+      <c r="N20" s="2">
         <v>428.46765475640666</v>
       </c>
-      <c r="O20" s="3">
+      <c r="O20" s="2">
         <v>16.54202005166532</v>
       </c>
-      <c r="P20" s="3">
+      <c r="P20" s="2">
         <v>1.9200539363419908</v>
       </c>
-      <c r="Q20" s="3">
+      <c r="Q20" s="2">
         <v>13.7218</v>
       </c>
-      <c r="R20" s="3">
+      <c r="R20" s="2">
         <v>81.10926274659087</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1">
         <v>2019</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>437.741235985068</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>1983.2747440965331</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>1.4509426812906687</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>1767.8042431911886</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>0.4425311463180663</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="2">
         <v>399.19905574062506</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="2">
         <v>177.47759195419528</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="2">
         <v>0.155660641686148</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="2">
         <v>1179.1098671585928</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K21" s="2">
         <v>18.225482252952812</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21" s="2">
         <v>668.0620131874147</v>
       </c>
-      <c r="M21" s="3">
+      <c r="M21" s="2">
         <v>22.347799045025106</v>
       </c>
-      <c r="N21" s="3">
+      <c r="N21" s="2">
         <v>474.8224095128133</v>
       </c>
-      <c r="O21" s="3">
+      <c r="O21" s="2">
         <v>27.954040103330644</v>
       </c>
-      <c r="P21" s="3">
+      <c r="P21" s="2">
         <v>2.0053078726839817</v>
       </c>
-      <c r="Q21" s="3">
+      <c r="Q21" s="2">
         <v>13.7218</v>
       </c>
-      <c r="R21" s="3">
+      <c r="R21" s="2">
         <v>104.49163348358094</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1">
         <v>2020</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>433.308564927602</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>1941.5429511447996</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>2.176414021936003</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>1804.3199172867828</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>0.6637967194770994</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="2">
         <v>421.95613361093757</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="2">
         <v>204.5453879312929</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="2">
         <v>0.23349096252922197</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="2">
         <v>1218.3365507378892</v>
       </c>
-      <c r="K22" s="3">
+      <c r="K22" s="2">
         <v>20.967873379429218</v>
       </c>
-      <c r="L22" s="3">
+      <c r="L22" s="2">
         <v>749.236919781122</v>
       </c>
-      <c r="M22" s="3">
+      <c r="M22" s="2">
         <v>29.02169856753766</v>
       </c>
-      <c r="N22" s="3">
+      <c r="N22" s="2">
         <v>521.1771642692199</v>
       </c>
-      <c r="O22" s="3">
+      <c r="O22" s="2">
         <v>39.366060154995964</v>
       </c>
-      <c r="P22" s="3">
+      <c r="P22" s="2">
         <v>2.0905618090259726</v>
       </c>
-      <c r="Q22" s="3">
+      <c r="Q22" s="2">
         <v>24.01316</v>
       </c>
-      <c r="R22" s="3">
+      <c r="R22" s="2">
         <v>123.34800469896021</v>
       </c>
     </row>
@@ -1700,55 +1697,55 @@
       <c r="A23" s="1">
         <v>2021</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>428.875893870136</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>1899.8111581930661</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>2.9018853625813374</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>1840.835591382377</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>0.8850622926361326</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="2">
         <v>444.7132114812501</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="2">
         <v>231.61318390839054</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="2">
         <v>0.311321283372296</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="2">
         <v>1257.5632343171856</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K23" s="2">
         <v>23.710264505905624</v>
       </c>
-      <c r="L23" s="3">
+      <c r="L23" s="2">
         <v>830.4118263748293</v>
       </c>
-      <c r="M23" s="3">
+      <c r="M23" s="2">
         <v>35.69559809005021</v>
       </c>
-      <c r="N23" s="3">
+      <c r="N23" s="2">
         <v>567.5319190256266</v>
       </c>
-      <c r="O23" s="3">
+      <c r="O23" s="2">
         <v>50.778080206661286</v>
       </c>
-      <c r="P23" s="3">
+      <c r="P23" s="2">
         <v>2.1758157453679634</v>
       </c>
-      <c r="Q23" s="3">
+      <c r="Q23" s="2">
         <v>24.01316</v>
       </c>
-      <c r="R23" s="3">
+      <c r="R23" s="2">
         <v>159.68265376256156</v>
       </c>
     </row>
@@ -1756,55 +1753,55 @@
       <c r="A24" s="1">
         <v>2022</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>424.44322281267</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>1858.0793652413327</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>3.627356703226672</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>1877.3512654779713</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <v>1.1063278657951656</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="2">
         <v>467.4702893515626</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="2">
         <v>258.68097988548817</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="2">
         <v>0.38915160421537</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="2">
         <v>1296.789917896482</v>
       </c>
-      <c r="K24" s="3">
+      <c r="K24" s="2">
         <v>26.45265563238203</v>
       </c>
-      <c r="L24" s="3">
+      <c r="L24" s="2">
         <v>911.5867329685366</v>
       </c>
-      <c r="M24" s="3">
+      <c r="M24" s="2">
         <v>42.36949761256277</v>
       </c>
-      <c r="N24" s="3">
+      <c r="N24" s="2">
         <v>613.8866737820333</v>
       </c>
-      <c r="O24" s="3">
+      <c r="O24" s="2">
         <v>62.19010025832661</v>
       </c>
-      <c r="P24" s="3">
+      <c r="P24" s="2">
         <v>2.2610696817099543</v>
       </c>
-      <c r="Q24" s="3">
+      <c r="Q24" s="2">
         <v>34.30451</v>
       </c>
-      <c r="R24" s="3">
+      <c r="R24" s="2">
         <v>194.6849395800611</v>
       </c>
     </row>
@@ -1812,55 +1809,55 @@
       <c r="A25" s="1">
         <v>2023</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>420.010551755204</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>1816.3475722895992</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>4.352828043872006</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>1913.8669395735656</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <v>1.3275934389541988</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="2">
         <v>490.2273672218751</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="2">
         <v>285.74877586258583</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="2">
         <v>0.466981925058444</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="2">
         <v>1336.0166014757783</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K25" s="2">
         <v>29.195046758858435</v>
       </c>
-      <c r="L25" s="3">
+      <c r="L25" s="2">
         <v>992.7616395622439</v>
       </c>
-      <c r="M25" s="3">
+      <c r="M25" s="2">
         <v>49.043397135075324</v>
       </c>
-      <c r="N25" s="3">
+      <c r="N25" s="2">
         <v>660.24142853844</v>
       </c>
-      <c r="O25" s="3">
+      <c r="O25" s="2">
         <v>73.60212030999193</v>
       </c>
-      <c r="P25" s="3">
+      <c r="P25" s="2">
         <v>2.346323618051945</v>
       </c>
-      <c r="Q25" s="3">
+      <c r="Q25" s="2">
         <v>44.59586</v>
       </c>
-      <c r="R25" s="3">
+      <c r="R25" s="2">
         <v>209.10003431784133</v>
       </c>
     </row>
@@ -1868,55 +1865,55 @@
       <c r="A26" s="1">
         <v>2024</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>415.577880697738</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>1774.6157793378657</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>5.07829938451734</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>1950.3826136691598</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="2">
         <v>1.548859012113232</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="2">
         <v>512.9844450921877</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="2">
         <v>312.8165718396835</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="2">
         <v>0.544812245901518</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="2">
         <v>1375.2432850550747</v>
       </c>
-      <c r="K26" s="3">
+      <c r="K26" s="2">
         <v>31.93743788533484</v>
       </c>
-      <c r="L26" s="3">
+      <c r="L26" s="2">
         <v>1073.9365461559512</v>
       </c>
-      <c r="M26" s="3">
+      <c r="M26" s="2">
         <v>55.71729665758788</v>
       </c>
-      <c r="N26" s="3">
+      <c r="N26" s="2">
         <v>706.5961832948467</v>
       </c>
-      <c r="O26" s="3">
+      <c r="O26" s="2">
         <v>85.01414036165725</v>
       </c>
-      <c r="P26" s="3">
+      <c r="P26" s="2">
         <v>2.431577554393936</v>
       </c>
-      <c r="Q26" s="3">
+      <c r="Q26" s="2">
         <v>65.17856</v>
       </c>
-      <c r="R26" s="3">
+      <c r="R26" s="2">
         <v>215.8894407823973</v>
       </c>
     </row>
@@ -1924,55 +1921,55 @@
       <c r="A27" s="1">
         <v>2025</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>411.14520964027207</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>1732.8839863861322</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>5.803770725162675</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>1986.8982877647538</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="2">
         <v>1.7701245852722651</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="2">
         <v>535.7415229625002</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="2">
         <v>339.8843678167811</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="2">
         <v>0.622642566744592</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="2">
         <v>1414.4699686343704</v>
       </c>
-      <c r="K27" s="3">
+      <c r="K27" s="2">
         <v>34.67982901181125</v>
       </c>
-      <c r="L27" s="3">
+      <c r="L27" s="2">
         <v>1155.1114527496584</v>
       </c>
-      <c r="M27" s="3">
+      <c r="M27" s="2">
         <v>62.39119618010043</v>
       </c>
-      <c r="N27" s="3">
+      <c r="N27" s="2">
         <v>752.9509380512533</v>
       </c>
-      <c r="O27" s="3">
+      <c r="O27" s="2">
         <v>96.42616041332258</v>
       </c>
-      <c r="P27" s="3">
+      <c r="P27" s="2">
         <v>2.5168314907359264</v>
       </c>
-      <c r="Q27" s="3">
+      <c r="Q27" s="2">
         <v>85.76127</v>
       </c>
-      <c r="R27" s="3">
+      <c r="R27" s="2">
         <v>225.63210621617154</v>
       </c>
     </row>
@@ -1980,55 +1977,55 @@
       <c r="A28" s="1">
         <v>2026</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>395.12182346903865</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>1664.6508966225579</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>13.10456326885318</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>1990.3278976013876</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="2">
         <v>5.756116837532743</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="2">
         <v>559.7473351253218</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="2">
         <v>353.4955346705021</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28" s="2">
         <v>0.8451485172367</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="2">
         <v>1446.8916547288227</v>
       </c>
-      <c r="K28" s="3">
+      <c r="K28" s="2">
         <v>37.80890863231117</v>
       </c>
-      <c r="L28" s="3">
+      <c r="L28" s="2">
         <v>1256.0330144775614</v>
       </c>
-      <c r="M28" s="3">
+      <c r="M28" s="2">
         <v>74.21796475223657</v>
       </c>
-      <c r="N28" s="3">
+      <c r="N28" s="2">
         <v>834.8283496524946</v>
       </c>
-      <c r="O28" s="3">
+      <c r="O28" s="2">
         <v>117.76318823855544</v>
       </c>
-      <c r="P28" s="3">
+      <c r="P28" s="2">
         <v>3.395462334748371</v>
       </c>
-      <c r="Q28" s="3">
+      <c r="Q28" s="2">
         <v>116.6353</v>
       </c>
-      <c r="R28" s="3">
+      <c r="R28" s="2">
         <v>228.35535877789854</v>
       </c>
     </row>
@@ -2036,55 +2033,55 @@
       <c r="A29" s="1">
         <v>2027</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>379.0984372978052</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>1596.4178068589836</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>20.405355812543686</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <v>1993.7575074380213</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="2">
         <v>9.742109089793221</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="2">
         <v>583.7531472881434</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="2">
         <v>367.10670152422307</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="2">
         <v>1.0676544677288082</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="2">
         <v>1479.313340823275</v>
       </c>
-      <c r="K29" s="3">
+      <c r="K29" s="2">
         <v>40.937988252811095</v>
       </c>
-      <c r="L29" s="3">
+      <c r="L29" s="2">
         <v>1356.9545762054645</v>
       </c>
-      <c r="M29" s="3">
+      <c r="M29" s="2">
         <v>86.04473332437271</v>
       </c>
-      <c r="N29" s="3">
+      <c r="N29" s="2">
         <v>916.7057612537359</v>
       </c>
-      <c r="O29" s="3">
+      <c r="O29" s="2">
         <v>139.1002160637883</v>
       </c>
-      <c r="P29" s="3">
+      <c r="P29" s="2">
         <v>4.274093178760816</v>
       </c>
-      <c r="Q29" s="3">
+      <c r="Q29" s="2">
         <v>137.218</v>
       </c>
-      <c r="R29" s="3">
+      <c r="R29" s="2">
         <v>244.99486557292815</v>
       </c>
     </row>
@@ -2092,55 +2089,55 @@
       <c r="A30" s="1">
         <v>2028</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>363.0750511265718</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="2">
         <v>1528.1847170954093</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="2">
         <v>27.70614835623419</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <v>1997.187117274655</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="2">
         <v>13.728101342053698</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="2">
         <v>607.758959450965</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="2">
         <v>380.71786837794406</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="2">
         <v>1.2901604182209163</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="2">
         <v>1511.7350269177273</v>
       </c>
-      <c r="K30" s="3">
+      <c r="K30" s="2">
         <v>44.06706787331102</v>
       </c>
-      <c r="L30" s="3">
+      <c r="L30" s="2">
         <v>1457.8761379333675</v>
       </c>
-      <c r="M30" s="3">
+      <c r="M30" s="2">
         <v>97.87150189650886</v>
       </c>
-      <c r="N30" s="3">
+      <c r="N30" s="2">
         <v>998.5831728549772</v>
       </c>
-      <c r="O30" s="3">
+      <c r="O30" s="2">
         <v>160.43724388902118</v>
       </c>
-      <c r="P30" s="3">
+      <c r="P30" s="2">
         <v>5.15272402277326</v>
       </c>
-      <c r="Q30" s="3">
+      <c r="Q30" s="2">
         <v>168.0921</v>
       </c>
-      <c r="R30" s="3">
+      <c r="R30" s="2">
         <v>255.35900191378894</v>
       </c>
     </row>
@@ -2148,55 +2145,55 @@
       <c r="A31" s="1">
         <v>2029</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>347.05166495533837</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="2">
         <v>1459.951627331835</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="2">
         <v>35.0069408999247</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <v>2000.6167271112888</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="2">
         <v>17.714093594314175</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="2">
         <v>631.7647716137866</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="2">
         <v>394.32903523166505</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31" s="2">
         <v>1.5126663687130244</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="2">
         <v>1544.1567130121796</v>
       </c>
-      <c r="K31" s="3">
+      <c r="K31" s="2">
         <v>47.19614749381094</v>
       </c>
-      <c r="L31" s="3">
+      <c r="L31" s="2">
         <v>1558.7976996612706</v>
       </c>
-      <c r="M31" s="3">
+      <c r="M31" s="2">
         <v>109.698270468645</v>
       </c>
-      <c r="N31" s="3">
+      <c r="N31" s="2">
         <v>1080.4605844562186</v>
       </c>
-      <c r="O31" s="3">
+      <c r="O31" s="2">
         <v>181.77427171425404</v>
       </c>
-      <c r="P31" s="3">
+      <c r="P31" s="2">
         <v>6.031354866785704</v>
       </c>
-      <c r="Q31" s="3">
+      <c r="Q31" s="2">
         <v>198.9661</v>
       </c>
-      <c r="R31" s="3">
+      <c r="R31" s="2">
         <v>270.17257078550404</v>
       </c>
     </row>
@@ -2204,55 +2201,55 @@
       <c r="A32" s="1">
         <v>2030</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>331.0282787841048</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <v>1391.7185375682607</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="2">
         <v>42.3077334436152</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="2">
         <v>2004.0463369479228</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="2">
         <v>21.700085846574652</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32" s="2">
         <v>655.7705837766083</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="2">
         <v>407.940202085386</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32" s="2">
         <v>1.7351723192051325</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="2">
         <v>1576.5783991066323</v>
       </c>
-      <c r="K32" s="3">
+      <c r="K32" s="2">
         <v>50.32522711431087</v>
       </c>
-      <c r="L32" s="3">
+      <c r="L32" s="2">
         <v>1659.7192613891732</v>
       </c>
-      <c r="M32" s="3">
+      <c r="M32" s="2">
         <v>121.52503904078114</v>
       </c>
-      <c r="N32" s="3">
+      <c r="N32" s="2">
         <v>1162.33799605746</v>
       </c>
-      <c r="O32" s="3">
+      <c r="O32" s="2">
         <v>203.1112995394869</v>
       </c>
-      <c r="P32" s="3">
+      <c r="P32" s="2">
         <v>6.909985710798149</v>
       </c>
-      <c r="Q32" s="3">
+      <c r="Q32" s="2">
         <v>240.1316</v>
       </c>
-      <c r="R32" s="3">
+      <c r="R32" s="2">
         <v>279.6240256948843</v>
       </c>
     </row>
@@ -2260,55 +2257,55 @@
       <c r="A33" s="1">
         <v>2031</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>318.61655368587674</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="2">
         <v>1271.9089256496063</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="2">
         <v>61.270662102171954</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="2">
         <v>1989.063506959898</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="2">
         <v>31.857328025775768</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G33" s="2">
         <v>674.6679984674018</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="2">
         <v>433.1898270589194</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I33" s="2">
         <v>3.264183851104425</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="2">
         <v>1599.3189812713588</v>
       </c>
-      <c r="K33" s="3">
+      <c r="K33" s="2">
         <v>54.20103032361668</v>
       </c>
-      <c r="L33" s="3">
+      <c r="L33" s="2">
         <v>1742.3888753200713</v>
       </c>
-      <c r="M33" s="3">
+      <c r="M33" s="2">
         <v>135.9098174753663</v>
       </c>
-      <c r="N33" s="3">
+      <c r="N33" s="2">
         <v>1284.1216460447215</v>
       </c>
-      <c r="O33" s="3">
+      <c r="O33" s="2">
         <v>237.0985136141078</v>
       </c>
-      <c r="P33" s="3">
+      <c r="P33" s="2">
         <v>9.404211737483596</v>
       </c>
-      <c r="Q33" s="3">
+      <c r="Q33" s="2">
         <v>271.0056</v>
       </c>
-      <c r="R33" s="3">
+      <c r="R33" s="2">
         <v>304.82821474215456</v>
       </c>
     </row>
@@ -2316,55 +2313,55 @@
       <c r="A34" s="1">
         <v>2032</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>306.20482858764865</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <v>1152.099313730952</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="2">
         <v>80.2335907607287</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="2">
         <v>1974.0806769718731</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="2">
         <v>42.014570204976884</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34" s="2">
         <v>693.5654131581954</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="2">
         <v>458.4394520324528</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34" s="2">
         <v>4.7931953830037175</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="2">
         <v>1622.0595634360852</v>
       </c>
-      <c r="K34" s="3">
+      <c r="K34" s="2">
         <v>58.076833532922485</v>
       </c>
-      <c r="L34" s="3">
+      <c r="L34" s="2">
         <v>1825.0584892509694</v>
       </c>
-      <c r="M34" s="3">
+      <c r="M34" s="2">
         <v>150.29459590995148</v>
       </c>
-      <c r="N34" s="3">
+      <c r="N34" s="2">
         <v>1405.905296031983</v>
       </c>
-      <c r="O34" s="3">
+      <c r="O34" s="2">
         <v>271.0857276887287</v>
       </c>
-      <c r="P34" s="3">
+      <c r="P34" s="2">
         <v>11.898437764169044</v>
       </c>
-      <c r="Q34" s="3">
+      <c r="Q34" s="2">
         <v>322.4624</v>
       </c>
-      <c r="R34" s="3">
+      <c r="R34" s="2">
         <v>315.5000689144865</v>
       </c>
     </row>
@@ -2372,55 +2369,55 @@
       <c r="A35" s="1">
         <v>2033</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <v>293.79310348942056</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="2">
         <v>1032.2897018122976</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="2">
         <v>99.19651941928547</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="2">
         <v>1959.0978469838483</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="2">
         <v>52.171812384178</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35" s="2">
         <v>712.4628278489889</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H35" s="2">
         <v>483.6890770059862</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35" s="2">
         <v>6.32220691490301</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="2">
         <v>1644.8001456008117</v>
       </c>
-      <c r="K35" s="3">
+      <c r="K35" s="2">
         <v>61.95263674222829</v>
       </c>
-      <c r="L35" s="3">
+      <c r="L35" s="2">
         <v>1907.7281031818675</v>
       </c>
-      <c r="M35" s="3">
+      <c r="M35" s="2">
         <v>164.67937434453665</v>
       </c>
-      <c r="N35" s="3">
+      <c r="N35" s="2">
         <v>1527.6889460192444</v>
       </c>
-      <c r="O35" s="3">
+      <c r="O35" s="2">
         <v>305.0729417633496</v>
       </c>
-      <c r="P35" s="3">
+      <c r="P35" s="2">
         <v>14.392663790854492</v>
       </c>
-      <c r="Q35" s="3">
+      <c r="Q35" s="2">
         <v>353.3364</v>
       </c>
-      <c r="R35" s="3">
+      <c r="R35" s="2">
         <v>353.45799331940304</v>
       </c>
     </row>
@@ -2428,55 +2425,55 @@
       <c r="A36" s="1">
         <v>2034</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <v>281.38137839119247</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="2">
         <v>912.4800898936431</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="2">
         <v>118.15944807784223</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="2">
         <v>1944.1150169958235</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="2">
         <v>62.32905456337912</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G36" s="2">
         <v>731.3602425397825</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H36" s="2">
         <v>508.9387019795196</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I36" s="2">
         <v>7.851218446802302</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36" s="2">
         <v>1667.5407277655381</v>
       </c>
-      <c r="K36" s="3">
+      <c r="K36" s="2">
         <v>65.8284399515341</v>
       </c>
-      <c r="L36" s="3">
+      <c r="L36" s="2">
         <v>1990.3977171127656</v>
       </c>
-      <c r="M36" s="3">
+      <c r="M36" s="2">
         <v>179.06415277912183</v>
       </c>
-      <c r="N36" s="3">
+      <c r="N36" s="2">
         <v>1649.472596006506</v>
       </c>
-      <c r="O36" s="3">
+      <c r="O36" s="2">
         <v>339.0601558379705</v>
       </c>
-      <c r="P36" s="3">
+      <c r="P36" s="2">
         <v>16.886889817539938</v>
       </c>
-      <c r="Q36" s="3">
+      <c r="Q36" s="2">
         <v>404.7932</v>
       </c>
-      <c r="R36" s="3">
+      <c r="R36" s="2">
         <v>378.2596264111574</v>
       </c>
     </row>
@@ -2484,55 +2481,55 @@
       <c r="A37" s="1">
         <v>2035</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>268.96965329296444</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="2">
         <v>792.6704779749884</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="2">
         <v>137.122376736399</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="2">
         <v>1929.1321870077982</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="2">
         <v>72.48629674258024</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G37" s="2">
         <v>750.2576572305762</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H37" s="2">
         <v>534.1883269530529</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I37" s="2">
         <v>9.380229978701594</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J37" s="2">
         <v>1690.2813099302648</v>
       </c>
-      <c r="K37" s="3">
+      <c r="K37" s="2">
         <v>69.7042431608399</v>
       </c>
-      <c r="L37" s="3">
+      <c r="L37" s="2">
         <v>2073.067331043664</v>
       </c>
-      <c r="M37" s="3">
+      <c r="M37" s="2">
         <v>193.44893121370706</v>
       </c>
-      <c r="N37" s="3">
+      <c r="N37" s="2">
         <v>1771.256245993767</v>
       </c>
-      <c r="O37" s="3">
+      <c r="O37" s="2">
         <v>373.04736991259136</v>
       </c>
-      <c r="P37" s="3">
+      <c r="P37" s="2">
         <v>19.381115844225388</v>
       </c>
-      <c r="Q37" s="3">
+      <c r="Q37" s="2">
         <v>456.25</v>
       </c>
-      <c r="R37" s="3">
+      <c r="R37" s="2">
         <v>411.28903928240084</v>
       </c>
     </row>
@@ -2540,55 +2537,55 @@
       <c r="A38" s="1">
         <v>2036</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>257.8886630390795</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="2">
         <v>712.8014111717954</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="2">
         <v>163.0304422028786</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="2">
         <v>1900.305055845075</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="2">
         <v>87.13550884079838</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38" s="2">
         <v>768.4618865441644</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="2">
         <v>568.8132683197149</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38" s="2">
         <v>14.302374331843215</v>
       </c>
-      <c r="J38" s="3">
+      <c r="J38" s="2">
         <v>1724.8882115095237</v>
       </c>
-      <c r="K38" s="3">
+      <c r="K38" s="2">
         <v>73.95236371413755</v>
       </c>
-      <c r="L38" s="3">
+      <c r="L38" s="2">
         <v>2143.7307504027617</v>
       </c>
-      <c r="M38" s="3">
+      <c r="M38" s="2">
         <v>208.21991084504594</v>
       </c>
-      <c r="N38" s="3">
+      <c r="N38" s="2">
         <v>1925.0831324718408</v>
       </c>
-      <c r="O38" s="3">
+      <c r="O38" s="2">
         <v>411.4662395602194</v>
       </c>
-      <c r="P38" s="3">
+      <c r="P38" s="2">
         <v>23.983266195308822</v>
       </c>
-      <c r="Q38" s="3">
+      <c r="Q38" s="2">
         <v>528.2894</v>
       </c>
-      <c r="R38" s="3">
+      <c r="R38" s="2">
         <v>432.85135486888146</v>
       </c>
     </row>
@@ -2596,55 +2593,55 @@
       <c r="A39" s="1">
         <v>2037</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="2">
         <v>246.8076727851946</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="2">
         <v>632.9323443686023</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="2">
         <v>188.9385076693582</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="2">
         <v>1871.4779246823518</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39" s="2">
         <v>101.78472093901652</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G39" s="2">
         <v>786.6661158577525</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H39" s="2">
         <v>603.4382096863769</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I39" s="2">
         <v>19.224518684984837</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39" s="2">
         <v>1759.4951130887825</v>
       </c>
-      <c r="K39" s="3">
+      <c r="K39" s="2">
         <v>78.2004842674352</v>
       </c>
-      <c r="L39" s="3">
+      <c r="L39" s="2">
         <v>2214.3941697618593</v>
       </c>
-      <c r="M39" s="3">
+      <c r="M39" s="2">
         <v>222.99089047638483</v>
       </c>
-      <c r="N39" s="3">
+      <c r="N39" s="2">
         <v>2078.9100189499145</v>
       </c>
-      <c r="O39" s="3">
+      <c r="O39" s="2">
         <v>449.8851092078474</v>
       </c>
-      <c r="P39" s="3">
+      <c r="P39" s="2">
         <v>28.585416546392256</v>
       </c>
-      <c r="Q39" s="3">
+      <c r="Q39" s="2">
         <v>600.3289</v>
       </c>
-      <c r="R39" s="3">
+      <c r="R39" s="2">
         <v>464.51257553066034</v>
       </c>
     </row>
@@ -2652,55 +2649,55 @@
       <c r="A40" s="1">
         <v>2038</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="2">
         <v>235.72668253130968</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="2">
         <v>553.0632775654093</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="2">
         <v>214.8465731358378</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="2">
         <v>1842.6507935196287</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40" s="2">
         <v>116.43393303723467</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G40" s="2">
         <v>804.8703451713407</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H40" s="2">
         <v>638.063151053039</v>
       </c>
-      <c r="I40" s="3">
+      <c r="I40" s="2">
         <v>24.146663038126455</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="2">
         <v>1794.1020146680414</v>
       </c>
-      <c r="K40" s="3">
+      <c r="K40" s="2">
         <v>82.44860482073285</v>
       </c>
-      <c r="L40" s="3">
+      <c r="L40" s="2">
         <v>2285.057589120957</v>
       </c>
-      <c r="M40" s="3">
+      <c r="M40" s="2">
         <v>237.76187010772372</v>
       </c>
-      <c r="N40" s="3">
+      <c r="N40" s="2">
         <v>2232.7369054279884</v>
       </c>
-      <c r="O40" s="3">
+      <c r="O40" s="2">
         <v>488.3039788554754</v>
       </c>
-      <c r="P40" s="3">
+      <c r="P40" s="2">
         <v>33.18756689747569</v>
       </c>
-      <c r="Q40" s="3">
+      <c r="Q40" s="2">
         <v>672.3684</v>
       </c>
-      <c r="R40" s="3">
+      <c r="R40" s="2">
         <v>507.36241701753295</v>
       </c>
     </row>
@@ -2708,55 +2705,55 @@
       <c r="A41" s="1">
         <v>2039</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="2">
         <v>224.64569227742476</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="2">
         <v>473.19421076221624</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="2">
         <v>240.75463860231739</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="2">
         <v>1813.8236623569055</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="2">
         <v>131.0831451354528</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41" s="2">
         <v>823.0745744849288</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="2">
         <v>672.688092419701</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I41" s="2">
         <v>29.068807391268074</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J41" s="2">
         <v>1828.7089162473003</v>
       </c>
-      <c r="K41" s="3">
+      <c r="K41" s="2">
         <v>86.6967253740305</v>
       </c>
-      <c r="L41" s="3">
+      <c r="L41" s="2">
         <v>2355.7210084800545</v>
       </c>
-      <c r="M41" s="3">
+      <c r="M41" s="2">
         <v>252.5328497390626</v>
       </c>
-      <c r="N41" s="3">
+      <c r="N41" s="2">
         <v>2386.5637919060623</v>
       </c>
-      <c r="O41" s="3">
+      <c r="O41" s="2">
         <v>526.7228485031034</v>
       </c>
-      <c r="P41" s="3">
+      <c r="P41" s="2">
         <v>37.78971724855913</v>
       </c>
-      <c r="Q41" s="3">
+      <c r="Q41" s="2">
         <v>754.6992</v>
       </c>
-      <c r="R41" s="3">
+      <c r="R41" s="2">
         <v>552.3167574009021</v>
       </c>
     </row>
@@ -2764,55 +2761,55 @@
       <c r="A42" s="1">
         <v>2040</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="2">
         <v>213.56470202353984</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="2">
         <v>393.3251439590233</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="2">
         <v>266.6627040687969</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="2">
         <v>1784.996531194182</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="2">
         <v>145.73235723367094</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42" s="2">
         <v>841.2788037985172</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="2">
         <v>707.313033786363</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I42" s="2">
         <v>33.99095174440969</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="2">
         <v>1863.3158178265594</v>
       </c>
-      <c r="K42" s="3">
+      <c r="K42" s="2">
         <v>90.94484592732815</v>
       </c>
-      <c r="L42" s="3">
+      <c r="L42" s="2">
         <v>2426.3844278391516</v>
       </c>
-      <c r="M42" s="3">
+      <c r="M42" s="2">
         <v>267.30382937040144</v>
       </c>
-      <c r="N42" s="3">
+      <c r="N42" s="2">
         <v>2540.390678384136</v>
       </c>
-      <c r="O42" s="3">
+      <c r="O42" s="2">
         <v>565.1417181507313</v>
       </c>
-      <c r="P42" s="3">
+      <c r="P42" s="2">
         <v>42.39186759964256</v>
       </c>
-      <c r="Q42" s="3">
+      <c r="Q42" s="2">
         <v>816.4473</v>
       </c>
-      <c r="R42" s="3">
+      <c r="R42" s="2">
         <v>631.5870212693749</v>
       </c>
     </row>
@@ -2820,55 +2817,55 @@
       <c r="A43" s="1">
         <v>2041</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="2">
         <v>208.85944290099704</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="2">
         <v>341.93349777583916</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="2">
         <v>282.5292039879148</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="2">
         <v>1791.5434032451237</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43" s="2">
         <v>161.51268678167685</v>
       </c>
-      <c r="G43" s="3">
+      <c r="G43" s="2">
         <v>855.4484726486814</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43" s="2">
         <v>753.9547558908583</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I43" s="2">
         <v>47.12776623750233</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J43" s="2">
         <v>1896.8395507202204</v>
       </c>
-      <c r="K43" s="3">
+      <c r="K43" s="2">
         <v>97.01640191974326</v>
       </c>
-      <c r="L43" s="3">
+      <c r="L43" s="2">
         <v>2478.696082672022</v>
       </c>
-      <c r="M43" s="3">
+      <c r="M43" s="2">
         <v>282.24256293576707</v>
       </c>
-      <c r="N43" s="3">
+      <c r="N43" s="2">
         <v>2728.456146196794</v>
       </c>
-      <c r="O43" s="3">
+      <c r="O43" s="2">
         <v>601.2745189737135</v>
       </c>
-      <c r="P43" s="3">
+      <c r="P43" s="2">
         <v>52.36096806715996</v>
       </c>
-      <c r="Q43" s="3">
+      <c r="Q43" s="2">
         <v>888.4867</v>
       </c>
-      <c r="R43" s="3">
+      <c r="R43" s="2">
         <v>715.7809324654121</v>
       </c>
     </row>
@@ -2876,55 +2873,55 @@
       <c r="A44" s="1">
         <v>2042</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="2">
         <v>204.15418377845424</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="2">
         <v>290.541851592655</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="2">
         <v>298.39570390703267</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="2">
         <v>1798.0902752960656</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44" s="2">
         <v>177.29301632968276</v>
       </c>
-      <c r="G44" s="3">
+      <c r="G44" s="2">
         <v>869.6181414988457</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H44" s="2">
         <v>800.5964779953537</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I44" s="2">
         <v>60.26458073059497</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44" s="2">
         <v>1930.3632836138813</v>
       </c>
-      <c r="K44" s="3">
+      <c r="K44" s="2">
         <v>103.08795791215837</v>
       </c>
-      <c r="L44" s="3">
+      <c r="L44" s="2">
         <v>2531.0077375048922</v>
       </c>
-      <c r="M44" s="3">
+      <c r="M44" s="2">
         <v>297.1812965011327</v>
       </c>
-      <c r="N44" s="3">
+      <c r="N44" s="2">
         <v>2916.521614009452</v>
       </c>
-      <c r="O44" s="3">
+      <c r="O44" s="2">
         <v>637.4073197966957</v>
       </c>
-      <c r="P44" s="3">
+      <c r="P44" s="2">
         <v>62.330068534677366</v>
       </c>
-      <c r="Q44" s="3">
+      <c r="Q44" s="2">
         <v>991.4003</v>
       </c>
-      <c r="R44" s="3">
+      <c r="R44" s="2">
         <v>785.9571830188042</v>
       </c>
     </row>
@@ -2932,55 +2929,55 @@
       <c r="A45" s="1">
         <v>2043</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="2">
         <v>199.44892465591144</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="2">
         <v>239.15020540947089</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="2">
         <v>314.26220382615054</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="2">
         <v>1804.6371473470074</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45" s="2">
         <v>193.07334587768867</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G45" s="2">
         <v>883.78781034901</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H45" s="2">
         <v>847.238200099849</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I45" s="2">
         <v>73.40139522368762</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J45" s="2">
         <v>1963.8870165075423</v>
       </c>
-      <c r="K45" s="3">
+      <c r="K45" s="2">
         <v>109.15951390457349</v>
       </c>
-      <c r="L45" s="3">
+      <c r="L45" s="2">
         <v>2583.3193923377626</v>
       </c>
-      <c r="M45" s="3">
+      <c r="M45" s="2">
         <v>312.1200300664983</v>
       </c>
-      <c r="N45" s="3">
+      <c r="N45" s="2">
         <v>3104.58708182211</v>
       </c>
-      <c r="O45" s="3">
+      <c r="O45" s="2">
         <v>673.5401206196779</v>
       </c>
-      <c r="P45" s="3">
+      <c r="P45" s="2">
         <v>72.29916900219477</v>
       </c>
-      <c r="Q45" s="3">
+      <c r="Q45" s="2">
         <v>1104.605</v>
       </c>
-      <c r="R45" s="3">
+      <c r="R45" s="2">
         <v>864.5175818651219</v>
       </c>
     </row>
@@ -2988,55 +2985,55 @@
       <c r="A46" s="1">
         <v>2044</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="2">
         <v>194.74366553336864</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="2">
         <v>187.75855922628676</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="2">
         <v>330.1287037452684</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="2">
         <v>1811.1840193979492</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F46" s="2">
         <v>208.85367542569458</v>
       </c>
-      <c r="G46" s="3">
+      <c r="G46" s="2">
         <v>897.9574791991743</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H46" s="2">
         <v>893.8799222043443</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I46" s="2">
         <v>86.53820971678026</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J46" s="2">
         <v>1997.4107494012032</v>
       </c>
-      <c r="K46" s="3">
+      <c r="K46" s="2">
         <v>115.2310698969886</v>
       </c>
-      <c r="L46" s="3">
+      <c r="L46" s="2">
         <v>2635.631047170633</v>
       </c>
-      <c r="M46" s="3">
+      <c r="M46" s="2">
         <v>327.05876363186394</v>
       </c>
-      <c r="N46" s="3">
+      <c r="N46" s="2">
         <v>3292.652549634768</v>
       </c>
-      <c r="O46" s="3">
+      <c r="O46" s="2">
         <v>709.67292144266</v>
       </c>
-      <c r="P46" s="3">
+      <c r="P46" s="2">
         <v>82.26826946971218</v>
       </c>
-      <c r="Q46" s="3">
+      <c r="Q46" s="2">
         <v>1197.227</v>
       </c>
-      <c r="R46" s="3">
+      <c r="R46" s="2">
         <v>984.350864586592</v>
       </c>
     </row>
@@ -3044,55 +3041,55 @@
       <c r="A47" s="1">
         <v>2045</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="2">
         <v>190.03840641082587</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="2">
         <v>136.36691304310267</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="2">
         <v>345.9952036643864</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="2">
         <v>1817.7308914488913</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F47" s="2">
         <v>224.63400497370054</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G47" s="2">
         <v>912.1271480493388</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H47" s="2">
         <v>940.5216443088394</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I47" s="2">
         <v>99.6750242098729</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47" s="2">
         <v>2030.9344822948644</v>
       </c>
-      <c r="K47" s="3">
+      <c r="K47" s="2">
         <v>121.30262588940374</v>
       </c>
-      <c r="L47" s="3">
+      <c r="L47" s="2">
         <v>2687.9427020035037</v>
       </c>
-      <c r="M47" s="3">
+      <c r="M47" s="2">
         <v>341.9974971972295</v>
       </c>
-      <c r="N47" s="3">
+      <c r="N47" s="2">
         <v>3480.718017447426</v>
       </c>
-      <c r="O47" s="3">
+      <c r="O47" s="2">
         <v>745.8057222656423</v>
       </c>
-      <c r="P47" s="3">
+      <c r="P47" s="2">
         <v>92.23736993722957</v>
       </c>
-      <c r="Q47" s="3">
+      <c r="Q47" s="2">
         <v>1300.141</v>
       </c>
-      <c r="R47" s="3">
+      <c r="R47" s="2">
         <v>1116.8146649674977</v>
       </c>
     </row>
@@ -3100,55 +3097,55 @@
       <c r="A48" s="1">
         <v>2046</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="2">
         <v>188.46898854818838</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="2">
         <v>131.47032730733218</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="2">
         <v>333.5771007017385</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="2">
         <v>1780.6884324759403</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F48" s="2">
         <v>236.89367739793704</v>
       </c>
-      <c r="G48" s="3">
+      <c r="G48" s="2">
         <v>922.7391615010349</v>
       </c>
-      <c r="H48" s="3">
+      <c r="H48" s="2">
         <v>977.7162619554344</v>
       </c>
-      <c r="I48" s="3">
+      <c r="I48" s="2">
         <v>112.18498905454652</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48" s="2">
         <v>2063.3860178077234</v>
       </c>
-      <c r="K48" s="3">
+      <c r="K48" s="2">
         <v>126.07731840370765</v>
       </c>
-      <c r="L48" s="3">
+      <c r="L48" s="2">
         <v>2757.7255868203665</v>
       </c>
-      <c r="M48" s="3">
+      <c r="M48" s="2">
         <v>360.9628957085956</v>
       </c>
-      <c r="N48" s="3">
+      <c r="N48" s="2">
         <v>3669.4005477261</v>
       </c>
-      <c r="O48" s="3">
+      <c r="O48" s="2">
         <v>784.4760177361503</v>
       </c>
-      <c r="P48" s="3">
+      <c r="P48" s="2">
         <v>110.10606978687244</v>
       </c>
-      <c r="Q48" s="3">
+      <c r="Q48" s="2">
         <v>1382.472</v>
       </c>
-      <c r="R48" s="3">
+      <c r="R48" s="2">
         <v>1295.2571708198127</v>
       </c>
     </row>
@@ -3156,55 +3153,55 @@
       <c r="A49" s="1">
         <v>2047</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="2">
         <v>186.89957068555088</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="2">
         <v>126.57374157156168</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="2">
         <v>321.15899773909064</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="2">
         <v>1743.6459735029894</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F49" s="2">
         <v>249.15334982217354</v>
       </c>
-      <c r="G49" s="3">
+      <c r="G49" s="2">
         <v>933.3511749527311</v>
       </c>
-      <c r="H49" s="3">
+      <c r="H49" s="2">
         <v>1014.9108796020295</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I49" s="2">
         <v>124.69495389922014</v>
       </c>
-      <c r="J49" s="3">
+      <c r="J49" s="2">
         <v>2095.837553320582</v>
       </c>
-      <c r="K49" s="3">
+      <c r="K49" s="2">
         <v>130.85201091801156</v>
       </c>
-      <c r="L49" s="3">
+      <c r="L49" s="2">
         <v>2827.5084716372294</v>
       </c>
-      <c r="M49" s="3">
+      <c r="M49" s="2">
         <v>379.92829421996174</v>
       </c>
-      <c r="N49" s="3">
+      <c r="N49" s="2">
         <v>3858.0830780047736</v>
       </c>
-      <c r="O49" s="3">
+      <c r="O49" s="2">
         <v>823.1463132066583</v>
       </c>
-      <c r="P49" s="3">
+      <c r="P49" s="2">
         <v>127.9747696365153</v>
       </c>
-      <c r="Q49" s="3">
+      <c r="Q49" s="2">
         <v>1495.677</v>
       </c>
-      <c r="R49" s="3">
+      <c r="R49" s="2">
         <v>1470.9614105377389</v>
       </c>
     </row>
@@ -3212,55 +3209,55 @@
       <c r="A50" s="1">
         <v>2048</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="2">
         <v>185.3301528229134</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="2">
         <v>121.67715583579118</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="2">
         <v>308.74089477644276</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="2">
         <v>1706.6035145300384</v>
       </c>
-      <c r="F50" s="3">
+      <c r="F50" s="2">
         <v>261.41302224641004</v>
       </c>
-      <c r="G50" s="3">
+      <c r="G50" s="2">
         <v>943.9631884044272</v>
       </c>
-      <c r="H50" s="3">
+      <c r="H50" s="2">
         <v>1052.1054972486245</v>
       </c>
-      <c r="I50" s="3">
+      <c r="I50" s="2">
         <v>137.20491874389376</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J50" s="2">
         <v>2128.289088833441</v>
       </c>
-      <c r="K50" s="3">
+      <c r="K50" s="2">
         <v>135.62670343231548</v>
       </c>
-      <c r="L50" s="3">
+      <c r="L50" s="2">
         <v>2897.2913564540922</v>
       </c>
-      <c r="M50" s="3">
+      <c r="M50" s="2">
         <v>398.89369273132786</v>
       </c>
-      <c r="N50" s="3">
+      <c r="N50" s="2">
         <v>4046.7656082834474</v>
       </c>
-      <c r="O50" s="3">
+      <c r="O50" s="2">
         <v>861.8166086771663</v>
       </c>
-      <c r="P50" s="3">
+      <c r="P50" s="2">
         <v>145.84346948615817</v>
       </c>
-      <c r="Q50" s="3">
+      <c r="Q50" s="2">
         <v>1547.133</v>
       </c>
-      <c r="R50" s="3">
+      <c r="R50" s="2">
         <v>1739.586043428648</v>
       </c>
     </row>
@@ -3268,55 +3265,55 @@
       <c r="A51" s="1">
         <v>2049</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="2">
         <v>183.7607349602759</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="2">
         <v>116.78057010002068</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="2">
         <v>296.3227918137949</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E51" s="2">
         <v>1669.5610555570875</v>
       </c>
-      <c r="F51" s="3">
+      <c r="F51" s="2">
         <v>273.67269467064654</v>
       </c>
-      <c r="G51" s="3">
+      <c r="G51" s="2">
         <v>954.5752018561234</v>
       </c>
-      <c r="H51" s="3">
+      <c r="H51" s="2">
         <v>1089.3001148952196</v>
       </c>
-      <c r="I51" s="3">
+      <c r="I51" s="2">
         <v>149.71488358856737</v>
       </c>
-      <c r="J51" s="3">
+      <c r="J51" s="2">
         <v>2160.7406243462997</v>
       </c>
-      <c r="K51" s="3">
+      <c r="K51" s="2">
         <v>140.4013959466194</v>
       </c>
-      <c r="L51" s="3">
+      <c r="L51" s="2">
         <v>2967.074241270955</v>
       </c>
-      <c r="M51" s="3">
+      <c r="M51" s="2">
         <v>417.859091242694</v>
       </c>
-      <c r="N51" s="3">
+      <c r="N51" s="2">
         <v>4235.448138562121</v>
       </c>
-      <c r="O51" s="3">
+      <c r="O51" s="2">
         <v>900.4869041476743</v>
       </c>
-      <c r="P51" s="3">
+      <c r="P51" s="2">
         <v>163.71216933580104</v>
       </c>
-      <c r="Q51" s="3">
+      <c r="Q51" s="2">
         <v>1660.338</v>
       </c>
-      <c r="R51" s="3">
+      <c r="R51" s="2">
         <v>1980.9962563303632</v>
       </c>
     </row>
@@ -3324,55 +3321,55 @@
       <c r="A52" s="1">
         <v>2050</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="2">
         <v>182.1913170976384</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="2">
         <v>111.88398436425018</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="2">
         <v>283.90468885114706</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52" s="2">
         <v>1632.518596584137</v>
       </c>
-      <c r="F52" s="3">
+      <c r="F52" s="2">
         <v>285.932367094883</v>
       </c>
-      <c r="G52" s="3">
+      <c r="G52" s="2">
         <v>965.1872153078195</v>
       </c>
-      <c r="H52" s="3">
+      <c r="H52" s="2">
         <v>1126.4947325418148</v>
       </c>
-      <c r="I52" s="3">
+      <c r="I52" s="2">
         <v>162.22484843324102</v>
       </c>
-      <c r="J52" s="3">
+      <c r="J52" s="2">
         <v>2193.192159859159</v>
       </c>
-      <c r="K52" s="3">
+      <c r="K52" s="2">
         <v>145.1760884609233</v>
       </c>
-      <c r="L52" s="3">
+      <c r="L52" s="2">
         <v>3036.8571260878175</v>
       </c>
-      <c r="M52" s="3">
+      <c r="M52" s="2">
         <v>436.8244897540602</v>
       </c>
-      <c r="N52" s="3">
+      <c r="N52" s="2">
         <v>4424.130668840796</v>
       </c>
-      <c r="O52" s="3">
+      <c r="O52" s="2">
         <v>939.1571996181825</v>
       </c>
-      <c r="P52" s="3">
+      <c r="P52" s="2">
         <v>181.58086918544387</v>
       </c>
-      <c r="Q52" s="3">
+      <c r="Q52" s="2">
         <v>1722.086</v>
       </c>
-      <c r="R52" s="3">
+      <c r="R52" s="2">
         <v>2312.124101662085</v>
       </c>
     </row>

</xml_diff>